<commit_message>
Write migration step in main.jl
</commit_message>
<xml_diff>
--- a/TN-SEIR-manual-sim.xlsx
+++ b/TN-SEIR-manual-sim.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqkligue\git\ASF-TN-SEIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uqkligue\git\ASF_TN_SEIR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E70F6506-709F-4467-B6C3-DE25BE9BD26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A06E299-78ED-4692-BEB7-714EC327447B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1440" windowWidth="21600" windowHeight="11175" xr2:uid="{8CE6783F-EA72-449F-83EE-1EA2C13D1D68}"/>
+    <workbookView xWindow="28695" yWindow="-1575" windowWidth="14610" windowHeight="15585" xr2:uid="{8CE6783F-EA72-449F-83EE-1EA2C13D1D68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +465,7 @@
   <dimension ref="B2:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,22 +544,22 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>20</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
         <v>24</v>
       </c>
       <c r="J4">
@@ -665,42 +672,42 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>3</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
         <f>G8</f>
         <v>3</v>
       </c>

</xml_diff>